<commit_message>
2.7.8 - Summer Heroes July 2025 + Leif & Melíai
</commit_message>
<xml_diff>
--- a/FEHSimulation/Spreadsheets/FEHSpecials.xlsx
+++ b/FEHSimulation/Spreadsheets/FEHSpecials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="539">
   <si>
     <t>Name</t>
   </si>
@@ -1641,6 +1641,21 @@
   </si>
   <si>
     <t>When Special triggers, boosts damage by 60% of unit's Res and neutralizes foe's "reduces damage by X%" effects from foe's non-Special skills. If unit's or foe's Special is ready, or unit's or foe's Special triggered before or during this combat, reduces damage from foe's next attack by 40% (once per combat; excluding area-of-effect Specials). If a Rally or movement Assist skill is used by unit, restores 20 HP to allies within 2 spaces of both unit and target ally after movement (including target ally; excluding unit), and neutralizes any [Penalty] on those allies (does not stack even if effect ranges of unit and target overlap), and grants another action to unit (additional action granted once per turn only; if another effect that grants additional action to unit has been triggered at the same time, this effect is also considered to have been triggered).</t>
+  </si>
+  <si>
+    <t>The True Njörun</t>
+  </si>
+  <si>
+    <t>Boosts damage by 50% of unit's Def when Special triggers.
+Enables [Canto (Ally 2, 2)].
+If unit initiates combat, after combat, if unit's Special triggered and unit survives, grants another action to unit, and also, if unit is not within 2 spaces of an ally, inflicts "restricts movement to 1 space" on unit and Pair Up cohort through their next action (once per turn; "within 2 spaces" is calculated based on the position of unit after triggering post-combat skill effects that change positioning).
+If unit's or foe's Special is ready, or unit's or foe's Special triggered before or during this combat, reduces damage from foe's next attack by 40% (once per combat; excluding area-of-effect Specials).</t>
+  </si>
+  <si>
+    <t>X!Leif</t>
+  </si>
+  <si>
+    <t>trueNjorun</t>
   </si>
 </sst>
 </file>
@@ -1959,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q163"/>
+  <dimension ref="A1:Q164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="J164" sqref="J164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,6 +8561,47 @@
       <c r="P163" s="1"/>
       <c r="Q163" s="1"/>
     </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C164" s="1">
+        <v>3</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F164" s="1">
+        <v>50</v>
+      </c>
+      <c r="G164" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="H164" s="1">
+        <v>0</v>
+      </c>
+      <c r="I164" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J164" s="1">
+        <v>0</v>
+      </c>
+      <c r="M164" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N164" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>